<commit_message>
Process overview and drivers without summation
Implement functionality without summation
Summation will be separated from tables into new table or statement

Add templates
</commit_message>
<xml_diff>
--- a/data/dictionary.xlsx
+++ b/data/dictionary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="979" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t xml:space="preserve">label used for calculation</t>
   </si>
@@ -40,28 +40,16 @@
     <t xml:space="preserve">Fahrzeug</t>
   </si>
   <si>
-    <t xml:space="preserve">dateStart</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Datum Beginn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dateEnd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Datum Ende</t>
-  </si>
-  <si>
-    <t xml:space="preserve">timeStart</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zeit Beginn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">timeEnd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zeit Ende</t>
+    <t xml:space="preserve">start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beginn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ende</t>
   </si>
   <si>
     <t xml:space="preserve">duration</t>
@@ -94,6 +82,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -115,6 +104,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -185,16 +175,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.2704081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -259,22 +249,6 @@
       </c>
       <c r="B8" s="0" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>